<commit_message>
Updated the project plan
</commit_message>
<xml_diff>
--- a/Project plan.xlsx
+++ b/Project plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>feature</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Marti</t>
+  </si>
+  <si>
+    <t>import external data</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -445,21 +448,21 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>8</v>
+      <c r="D2" s="1">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -467,27 +470,39 @@
       <c r="C3" s="1">
         <v>8</v>
       </c>
+      <c r="D3" s="1">
+        <v>16</v>
+      </c>
       <c r="E3" s="1">
         <v>8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1">
         <v>8</v>
       </c>
+      <c r="D4" s="1">
+        <v>16</v>
+      </c>
       <c r="E4" s="1">
         <v>8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
@@ -501,10 +516,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1">
         <v>8</v>
@@ -515,7 +530,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
@@ -527,37 +542,43 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1">
-        <v>12</v>
-      </c>
-      <c r="E9" s="1">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
       </c>
       <c r="E10" s="1">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
@@ -571,10 +592,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1">
         <v>4</v>
@@ -585,21 +606,27 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1">
         <v>4</v>
       </c>
+      <c r="D13" s="1">
+        <v>8</v>
+      </c>
       <c r="E13" s="1">
         <v>4</v>
+      </c>
+      <c r="F13" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>19</v>
@@ -608,6 +635,20 @@
         <v>4</v>
       </c>
       <c r="E14" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1">
         <v>4</v>
       </c>
     </row>

</xml_diff>